<commit_message>
Got rid of hubbytronics link
</commit_message>
<xml_diff>
--- a/BOM/RCS_R2_BOM.xlsx
+++ b/BOM/RCS_R2_BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serena\Documents\GitHub\Electrical-and-Software\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cornell_2016-2017\Rocketry\Electrical-and-Software\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7092"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>https://www.sparkfun.com/products/8533</t>
   </si>
   <si>
-    <t>http://www.hobbytronics.co.uk/eeprom-24lc256</t>
-  </si>
-  <si>
     <t>https://www.sparkfun.com/products/13762</t>
   </si>
   <si>
@@ -192,12 +189,15 @@
   </si>
   <si>
     <t>https://www.amazon.com/gp/product/B00WQ5DAXQ/ref=oh_aui_detailpage_o05_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/microchip-technology/24LC256-I-P/24LC256-I-P-ND/273431</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,22 +573,22 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.36328125" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="5" max="5" width="6.6328125" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>16</v>
@@ -600,7 +600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -611,7 +611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -619,24 +619,24 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -650,7 +650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -661,7 +661,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -675,7 +675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -683,13 +683,13 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -703,7 +703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -717,7 +717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -731,7 +731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -742,94 +742,94 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>12</v>
@@ -842,7 +842,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -850,13 +850,13 @@
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -870,7 +870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -878,67 +878,67 @@
         <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -949,13 +949,12 @@
     <hyperlink ref="D11" r:id="rId4"/>
     <hyperlink ref="D18" r:id="rId5"/>
     <hyperlink ref="D5" r:id="rId6"/>
-    <hyperlink ref="D21" r:id="rId7"/>
-    <hyperlink ref="D3" r:id="rId8"/>
-    <hyperlink ref="D19" r:id="rId9"/>
-    <hyperlink ref="D24" r:id="rId10"/>
-    <hyperlink ref="D17" r:id="rId11"/>
+    <hyperlink ref="D3" r:id="rId7"/>
+    <hyperlink ref="D19" r:id="rId8"/>
+    <hyperlink ref="D24" r:id="rId9"/>
+    <hyperlink ref="D17" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last additions to the BOM
</commit_message>
<xml_diff>
--- a/BOM/RCS_R2_BOM.xlsx
+++ b/BOM/RCS_R2_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>MPU Breakout</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/microchip-technology/24LC256-I-P/24LC256-I-P-ND/273431</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/atmel/ATMEGA328P-AUR/ATMEGA328P-AURCT-ND/3789455</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/invensense/MPU-9250/1428-1019-1-ND/4626450</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/kemet/C1206C106K4PACTU/399-5091-1-ND/1465625</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/kingbright/APT3216SURCK/754-1143-1-ND/1747860</t>
   </si>
 </sst>
 </file>
@@ -569,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,6 +619,9 @@
       <c r="C2">
         <v>2</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
@@ -618,8 +633,8 @@
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
+      <c r="D3" t="s">
+        <v>57</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -632,6 +647,12 @@
       <c r="B4" t="s">
         <v>30</v>
       </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
       <c r="E4" t="s">
         <v>18</v>
       </c>
@@ -657,6 +678,9 @@
       <c r="C6">
         <v>5</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
@@ -737,6 +761,9 @@
       </c>
       <c r="C12">
         <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
@@ -949,12 +976,13 @@
     <hyperlink ref="D11" r:id="rId4"/>
     <hyperlink ref="D18" r:id="rId5"/>
     <hyperlink ref="D5" r:id="rId6"/>
-    <hyperlink ref="D3" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId7"/>
     <hyperlink ref="D19" r:id="rId8"/>
     <hyperlink ref="D24" r:id="rId9"/>
     <hyperlink ref="D17" r:id="rId10"/>
+    <hyperlink ref="D6" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>